<commit_message>
base class is changed
</commit_message>
<xml_diff>
--- a/src/main/java/com/ebaysearch/Testdata/Testdata_ebay.xlsx
+++ b/src/main/java/com/ebaysearch/Testdata/Testdata_ebay.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium_projects\selenium_assignment_dummy\src\main\java\ebay\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\backup 12112019\jansi_javafiles_2\selenium_assignment\src\main\java\com\ebaysearch\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C334361-F344-46FD-9830-BB9303C9FB50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CB5184-DEBE-4AD1-9713-90D03500E1DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +433,7 @@
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -453,7 +453,7 @@
       <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
@@ -479,7 +479,7 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>2</v>
       </c>
       <c r="G2">
@@ -505,7 +505,7 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3">
@@ -531,7 +531,7 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>1</v>
       </c>
       <c r="G4">
@@ -557,7 +557,7 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5">

</xml_diff>